<commit_message>
add C++ script and change countVect to TFIDF
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinsu99/Desktop/RENE/flaky_tests_AI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD711B1-A659-CF49-99CE-EB8B430A1CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A471C9-337F-5544-9F0B-36E8310542F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="500" windowWidth="33080" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="23020" windowWidth="22820" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="70-30 normal" sheetId="1" r:id="rId1"/>
@@ -2366,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A50" sqref="A50:A57"/>
     </sheetView>
   </sheetViews>
@@ -4069,11 +4069,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666F141A-4ACA-0C49-8B35-C58E9F1E973C}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="K67" sqref="K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
@@ -11000,15 +11003,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="A66:A73"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
     <mergeCell ref="A74:A81"/>
     <mergeCell ref="A82:A89"/>
     <mergeCell ref="A146:A153"/>
@@ -11020,6 +11014,15 @@
     <mergeCell ref="A130:A137"/>
     <mergeCell ref="A138:A145"/>
     <mergeCell ref="A90:A97"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="A58:A65"/>
+    <mergeCell ref="A66:A73"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>